<commit_message>
Add tests on group view with TestCase
Add tests on group view with TestCase, and to support this an extension of IWebDriver.FindElements by ElementLocation object is added too
</commit_message>
<xml_diff>
--- a/TestOnTankLibrary/Data/Location.xlsx
+++ b/TestOnTankLibrary/Data/Location.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -51,6 +51,28 @@
     </r>
   </si>
   <si>
+    <t>Home.WWI</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t>http://www.tanklib.franklidev.com/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
     <t>Location</t>
   </si>
   <si>
@@ -70,6 +92,39 @@
   </si>
   <si>
     <t>.fa.fa-plus-square</t>
+  </si>
+  <si>
+    <t>Home.Group.WWI</t>
+  </si>
+  <si>
+    <t>LinkText</t>
+  </si>
+  <si>
+    <t>World War I</t>
+  </si>
+  <si>
+    <t>Home.Group.WWII</t>
+  </si>
+  <si>
+    <t>World War II</t>
+  </si>
+  <si>
+    <t>Home.Group.Interwar</t>
+  </si>
+  <si>
+    <t>Interwar</t>
+  </si>
+  <si>
+    <t>Home.Group.Modern</t>
+  </si>
+  <si>
+    <t>Modern</t>
+  </si>
+  <si>
+    <t>Home.List.Stages</t>
+  </si>
+  <si>
+    <t>#tanklist tr.clickable-row td:nth-child(3)</t>
   </si>
   <si>
     <t>Expected</t>
@@ -91,7 +146,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -125,13 +180,18 @@
       <name val="Times"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,12 +236,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="21"/>
+        <fgColor indexed="19"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="20"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="23"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -246,6 +318,61 @@
         <color indexed="14"/>
       </top>
       <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
         <color indexed="13"/>
       </bottom>
       <diagonal/>
@@ -298,13 +425,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="15"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="21"/>
+      </left>
+      <right style="thin">
+        <color indexed="21"/>
+      </right>
+      <top style="thin">
+        <color indexed="21"/>
       </top>
       <bottom style="thin">
         <color indexed="14"/>
@@ -313,16 +455,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="21"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="21"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="21"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="22"/>
       </bottom>
       <diagonal/>
     </border>
@@ -331,178 +473,103 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="21"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="22"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="21"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="21"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="21"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="21"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="21"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
       </right>
       <top style="thin">
         <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="16"/>
+        <color indexed="21"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="22"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="21"/>
       </right>
       <top style="thin">
         <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="16"/>
+        <color indexed="21"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="19"/>
+        <color indexed="21"/>
       </left>
       <right style="thin">
-        <color indexed="19"/>
+        <color indexed="21"/>
       </right>
       <top style="thin">
-        <color indexed="19"/>
+        <color indexed="21"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="21"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="19"/>
+        <color indexed="21"/>
       </left>
       <right style="thin">
-        <color indexed="19"/>
+        <color indexed="22"/>
       </right>
       <top style="thin">
-        <color indexed="19"/>
+        <color indexed="21"/>
       </top>
       <bottom style="thin">
-        <color indexed="20"/>
+        <color indexed="21"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="22"/>
       </left>
       <right style="thin">
-        <color indexed="19"/>
+        <color indexed="21"/>
       </right>
       <top style="thin">
-        <color indexed="20"/>
+        <color indexed="21"/>
       </top>
       <bottom style="thin">
-        <color indexed="19"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="19"/>
-      </left>
-      <right style="thin">
-        <color indexed="19"/>
-      </right>
-      <top style="thin">
-        <color indexed="20"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="19"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="19"/>
-      </left>
-      <right style="thin">
-        <color indexed="20"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="19"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="20"/>
-      </left>
-      <right style="thin">
-        <color indexed="19"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="19"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="19"/>
-      </left>
-      <right style="thin">
-        <color indexed="19"/>
-      </right>
-      <top style="thin">
-        <color indexed="19"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="19"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="19"/>
-      </left>
-      <right style="thin">
-        <color indexed="20"/>
-      </right>
-      <top style="thin">
-        <color indexed="19"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="19"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="20"/>
-      </left>
-      <right style="thin">
-        <color indexed="19"/>
-      </right>
-      <top style="thin">
-        <color indexed="19"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="19"/>
+        <color indexed="21"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,7 +579,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -561,67 +628,70 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -650,6 +720,8 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffcacaca"/>
+      <rgbColor rgb="ffe6e6e6"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
@@ -1760,7 +1832,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1771,12 +1843,12 @@
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s" s="3">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1787,7 +1859,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1807,7 +1879,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1841,9 +1913,21 @@
       <c r="D2" s="14"/>
       <c r="E2" s="15"/>
     </row>
+    <row r="3" ht="16.55" customHeight="1">
+      <c r="A3" t="s" s="16">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s" s="17">
+        <v>10</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="" tooltip="" display="http://www.tanklib.franklidev.com/"/>
+    <hyperlink ref="B3" r:id="rId2" location="" tooltip="" display="http://www.tanklib.franklidev.com/"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -1855,56 +1939,123 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="11.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="16.3516" style="16" customWidth="1"/>
-    <col min="3" max="3" width="27.0938" style="16" customWidth="1"/>
-    <col min="4" max="7" width="16.3516" style="16" customWidth="1"/>
-    <col min="8" max="256" width="16.3516" style="16" customWidth="1"/>
+    <col min="1" max="1" width="19.1484" style="21" customWidth="1"/>
+    <col min="2" max="2" width="16.3516" style="21" customWidth="1"/>
+    <col min="3" max="3" width="41.8828" style="21" customWidth="1"/>
+    <col min="4" max="7" width="16.3516" style="21" customWidth="1"/>
+    <col min="8" max="256" width="16.3516" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
-      <c r="A1" t="s" s="17">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s" s="17">
-        <v>11</v>
-      </c>
-      <c r="C1" t="s" s="17">
+      <c r="A1" t="s" s="22">
         <v>12</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="B1" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s" s="22">
+        <v>14</v>
+      </c>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s" s="20">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s" s="21">
+      <c r="A2" t="s" s="24">
         <v>15</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="B2" t="s" s="24">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s" s="24">
+        <v>17</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="23"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="A3" t="s" s="22">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s" s="22">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="22">
+        <v>20</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" ht="20.25" customHeight="1">
+      <c r="A4" t="s" s="24">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s" s="24">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s" s="24">
+        <v>22</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+    </row>
+    <row r="5" ht="20.25" customHeight="1">
+      <c r="A5" t="s" s="22">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s" s="22">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s" s="22">
+        <v>24</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" ht="20.25" customHeight="1">
+      <c r="A6" t="s" s="24">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s" s="24">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s" s="24">
+        <v>26</v>
+      </c>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" ht="20.25" customHeight="1">
+      <c r="A7" t="s" s="22">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s" s="22">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s" s="22">
+        <v>28</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -1936,81 +2087,81 @@
   <sheetData>
     <row r="1" ht="14.35" customHeight="1">
       <c r="A1" t="s" s="27">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s" s="27">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
     </row>
     <row r="2" ht="14.7" customHeight="1">
-      <c r="A2" t="s" s="19">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s" s="29">
-        <v>19</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="A2" t="s" s="29">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s" s="30">
+        <v>32</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" ht="14.35" customHeight="1">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" ht="14.05" customHeight="1">
-      <c r="A4" s="35"/>
-      <c r="B4" s="36"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" ht="14.05" customHeight="1">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
     </row>
     <row r="6" ht="14.05" customHeight="1">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
     </row>
     <row r="7" ht="14.05" customHeight="1">
-      <c r="A7" s="35"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
     </row>
     <row r="8" ht="14.05" customHeight="1">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
     </row>
     <row r="9" ht="14.05" customHeight="1">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
     </row>
     <row r="10" ht="14.05" customHeight="1">
-      <c r="A10" s="35"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="35"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Add test on click group All
</commit_message>
<xml_diff>
--- a/TestOnTankLibrary/Data/Location.xlsx
+++ b/TestOnTankLibrary/Data/Location.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>#tanklist tr.clickable-row td:nth-child(3)</t>
+  </si>
+  <si>
+    <t>Home.Group.All</t>
+  </si>
+  <si>
+    <t>All</t>
   </si>
   <si>
     <t>Expected</t>
@@ -1848,7 +1854,7 @@
     </row>
     <row r="13">
       <c r="B13" t="s" s="3">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1859,7 +1865,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1939,7 +1945,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2056,6 +2062,21 @@
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
       <c r="G7" s="23"/>
+    </row>
+    <row r="8" ht="20.25" customHeight="1">
+      <c r="A8" t="s" s="24">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s" s="24">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s" s="24">
+        <v>30</v>
+      </c>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -2090,7 +2111,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s" s="27">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -2098,10 +2119,10 @@
     </row>
     <row r="2" ht="14.7" customHeight="1">
       <c r="A2" t="s" s="29">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s" s="30">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="32"/>

</xml_diff>

<commit_message>
Add test cases on selecting row on tank list
Add 2 test cases on selecting different row on tank list to check the reflection of image and description area.
</commit_message>
<xml_diff>
--- a/TestOnTankLibrary/Data/Location.xlsx
+++ b/TestOnTankLibrary/Data/Location.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -131,6 +131,39 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Home.List.All.Data2.Name</t>
+  </si>
+  <si>
+    <t>XPath</t>
+  </si>
+  <si>
+    <t>//*[@id='tanklist']/tbody/tr[2]/td[2]</t>
+  </si>
+  <si>
+    <t>Home.List.All.Data2.Stage</t>
+  </si>
+  <si>
+    <t>//*[@id='tanklist']/tbody/tr[2]/td[3]</t>
+  </si>
+  <si>
+    <t>Home.List.All.Data3.Name</t>
+  </si>
+  <si>
+    <t>//*[@id='tanklist']/tbody/tr[3]/td[2]</t>
+  </si>
+  <si>
+    <t>Home.List.All.Data3.Type</t>
+  </si>
+  <si>
+    <t>//*[@id='tanklist']/tbody/tr[3]/td[4]</t>
+  </si>
+  <si>
+    <t>Home.Desc.Name</t>
+  </si>
+  <si>
+    <t>//*[@id='imganddesc_div']/div/h4</t>
   </si>
   <si>
     <t>Expected</t>
@@ -1854,7 +1887,7 @@
     </row>
     <row r="13">
       <c r="B13" t="s" s="3">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1865,7 +1898,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1945,13 +1978,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="11.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.1484" style="21" customWidth="1"/>
+    <col min="1" max="1" width="25.5859" style="21" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="21" customWidth="1"/>
     <col min="3" max="3" width="41.8828" style="21" customWidth="1"/>
     <col min="4" max="7" width="16.3516" style="21" customWidth="1"/>
@@ -2077,6 +2110,81 @@
       <c r="E8" s="25"/>
       <c r="F8" s="25"/>
       <c r="G8" s="25"/>
+    </row>
+    <row r="9" ht="20.25" customHeight="1">
+      <c r="A9" t="s" s="22">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s" s="22">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s" s="22">
+        <v>33</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" ht="20.25" customHeight="1">
+      <c r="A10" t="s" s="24">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s" s="24">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s" s="24">
+        <v>35</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" ht="20.25" customHeight="1">
+      <c r="A11" t="s" s="22">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s" s="22">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s" s="22">
+        <v>37</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+    </row>
+    <row r="12" ht="20.25" customHeight="1">
+      <c r="A12" t="s" s="24">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s" s="24">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s" s="24">
+        <v>39</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" ht="20.25" customHeight="1">
+      <c r="A13" t="s" s="22">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s" s="22">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s" s="22">
+        <v>41</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -2111,7 +2219,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s" s="27">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -2119,10 +2227,10 @@
     </row>
     <row r="2" ht="14.7" customHeight="1">
       <c r="A2" t="s" s="29">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s" s="30">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="32"/>

</xml_diff>

<commit_message>
Add test on displaying detail by clicking name of tank on the list
</commit_message>
<xml_diff>
--- a/TestOnTankLibrary/Data/Location.xlsx
+++ b/TestOnTankLibrary/Data/Location.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>//*[@id='imganddesc_div']/div/h4</t>
+  </si>
+  <si>
+    <t>Detail.Name</t>
+  </si>
+  <si>
+    <t>//dt[text()='Name']/following-sibling::dd[1]</t>
   </si>
   <si>
     <t>Expected</t>
@@ -1887,7 +1893,7 @@
     </row>
     <row r="13">
       <c r="B13" t="s" s="3">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1898,7 +1904,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1978,7 +1984,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2185,6 +2191,21 @@
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
+    </row>
+    <row r="14" ht="20.25" customHeight="1">
+      <c r="A14" t="s" s="24">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s" s="24">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s" s="24">
+        <v>43</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -2219,7 +2240,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s" s="27">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -2227,10 +2248,10 @@
     </row>
     <row r="2" ht="14.7" customHeight="1">
       <c r="A2" t="s" s="29">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s" s="30">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="32"/>

</xml_diff>

<commit_message>
Refine row number dependant element location to paramterized settings
</commit_message>
<xml_diff>
--- a/TestOnTankLibrary/Data/Location.xlsx
+++ b/TestOnTankLibrary/Data/Location.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -133,31 +133,25 @@
     <t>All</t>
   </si>
   <si>
-    <t>Home.List.All.Data2.Name</t>
+    <t>Home.List.All.Data.Name</t>
   </si>
   <si>
     <t>XPath</t>
   </si>
   <si>
-    <t>//*[@id='tanklist']/tbody/tr[2]/td[2]</t>
-  </si>
-  <si>
-    <t>Home.List.All.Data2.Stage</t>
-  </si>
-  <si>
-    <t>//*[@id='tanklist']/tbody/tr[2]/td[3]</t>
-  </si>
-  <si>
-    <t>Home.List.All.Data3.Name</t>
-  </si>
-  <si>
-    <t>//*[@id='tanklist']/tbody/tr[3]/td[2]</t>
-  </si>
-  <si>
-    <t>Home.List.All.Data3.Type</t>
-  </si>
-  <si>
-    <t>//*[@id='tanklist']/tbody/tr[3]/td[4]</t>
+    <t>//*[@id='tanklist']/tbody/tr[{0}]/td[2]</t>
+  </si>
+  <si>
+    <t>Home.List.All.Data.Stage</t>
+  </si>
+  <si>
+    <t>//*[@id='tanklist']/tbody/tr[{0}]/td[3]</t>
+  </si>
+  <si>
+    <t>Home.List.All.Data.Type</t>
+  </si>
+  <si>
+    <t>//*[@id='tanklist']/tbody/tr[{0}]/td[4]</t>
   </si>
   <si>
     <t>Home.Desc.Name</t>
@@ -170,6 +164,27 @@
   </si>
   <si>
     <t>//dt[text()='Name']/following-sibling::dd[1]</t>
+  </si>
+  <si>
+    <t>Home.List.All.Data.Btn.Edit</t>
+  </si>
+  <si>
+    <t>//*[@id='tanklist']/tbody/tr[{0}]/td[1]//i[@class='fa fa-edit']</t>
+  </si>
+  <si>
+    <t>Home.List.All.Data.Btn.Delete</t>
+  </si>
+  <si>
+    <t>//*[@id='tanklist']/tbody/tr[{0}]/td[1]//i[@class='fa fa-trash']</t>
+  </si>
+  <si>
+    <t>Edit.Name</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
   <si>
     <t>Expected</t>
@@ -1893,7 +1908,7 @@
     </row>
     <row r="13">
       <c r="B13" t="s" s="3">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1904,7 +1919,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1984,7 +1999,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1992,7 +2007,7 @@
   <cols>
     <col min="1" max="1" width="25.5859" style="21" customWidth="1"/>
     <col min="2" max="2" width="16.3516" style="21" customWidth="1"/>
-    <col min="3" max="3" width="41.8828" style="21" customWidth="1"/>
+    <col min="3" max="3" width="53.5703" style="21" customWidth="1"/>
     <col min="4" max="7" width="16.3516" style="21" customWidth="1"/>
     <col min="8" max="256" width="16.3516" style="21" customWidth="1"/>
   </cols>
@@ -2206,6 +2221,36 @@
       <c r="E14" s="25"/>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
+    </row>
+    <row r="15" ht="20.25" customHeight="1">
+      <c r="A15" t="s" s="22">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s" s="22">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s" s="22">
+        <v>45</v>
+      </c>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+    </row>
+    <row r="16" ht="20.25" customHeight="1">
+      <c r="A16" t="s" s="24">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s" s="24">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s" s="24">
+        <v>48</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -2240,7 +2285,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s" s="27">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -2248,10 +2293,10 @@
     </row>
     <row r="2" ht="14.7" customHeight="1">
       <c r="A2" t="s" s="29">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s" s="30">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="32"/>

</xml_diff>

<commit_message>
Add test cases for displaying delete page
</commit_message>
<xml_diff>
--- a/TestOnTankLibrary/Data/Location.xlsx
+++ b/TestOnTankLibrary/Data/Location.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Delete.Name</t>
+  </si>
+  <si>
+    <t>//form/div/h4</t>
   </si>
   <si>
     <t>Expected</t>
@@ -1908,7 +1914,7 @@
     </row>
     <row r="13">
       <c r="B13" t="s" s="3">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1919,7 +1925,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1999,7 +2005,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2251,6 +2257,21 @@
       <c r="E16" s="25"/>
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
+    </row>
+    <row r="17" ht="20.25" customHeight="1">
+      <c r="A17" t="s" s="22">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s" s="22">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s" s="22">
+        <v>50</v>
+      </c>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -2285,7 +2306,7 @@
         <v>12</v>
       </c>
       <c r="B1" t="s" s="27">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -2293,10 +2314,10 @@
     </row>
     <row r="2" ht="14.7" customHeight="1">
       <c r="A2" t="s" s="29">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s" s="30">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="32"/>

</xml_diff>

<commit_message>
Add test on clicking on page number
Add test on clicking on page number and adjust the test on edit button after TankLibrary changed to not allow to change default tanks.
</commit_message>
<xml_diff>
--- a/TestOnTankLibrary/Data/Location.xlsx
+++ b/TestOnTankLibrary/Data/Location.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -61,15 +61,30 @@
         <color indexed="11"/>
         <rFont val="Times"/>
       </rPr>
-      <t>http://www.tanklib.franklidev.com/</t>
+      <t>http://www.tanklib.franklidev.com/1</t>
+    </r>
+  </si>
+  <si>
+    <t>Home.Page</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t>http://www.tanklib.franklidev.com/Page</t>
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="18"/>
+        <rFont val="Times"/>
       </rPr>
-      <t>1</t>
+      <t>{0}?curindex=0</t>
     </r>
   </si>
   <si>
@@ -191,6 +206,24 @@
   </si>
   <si>
     <t>//form/div/h4</t>
+  </si>
+  <si>
+    <t>Home.List.Page.Enabled</t>
+  </si>
+  <si>
+    <t>//a[text()='{0}' and contains(@class, 'btn btn-default')]</t>
+  </si>
+  <si>
+    <t>Home.List.Page.Disabled</t>
+  </si>
+  <si>
+    <t>//span[text()='{0}' and contains(@class, 'disabled btn btn-default')]</t>
+  </si>
+  <si>
+    <t>FunctionPage.Btn.BackToList</t>
+  </si>
+  <si>
+    <t>//a[text()='Back to List']</t>
   </si>
   <si>
     <t>Expected</t>
@@ -212,7 +245,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -243,6 +276,12 @@
       <u val="single"/>
       <sz val="12"/>
       <color indexed="11"/>
+      <name val="Times"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="18"/>
       <name val="Times"/>
     </font>
     <font>
@@ -296,12 +335,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="18"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="19"/>
         <bgColor auto="1"/>
       </patternFill>
@@ -314,7 +347,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="23"/>
+        <fgColor indexed="21"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="24"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -506,13 +545,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </left>
       <right style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </right>
       <top style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </top>
       <bottom style="thin">
         <color indexed="14"/>
@@ -521,13 +560,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </left>
       <right style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </right>
       <top style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="23"/>
       </top>
       <bottom style="thin">
         <color indexed="22"/>
@@ -536,37 +590,37 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="22"/>
       </left>
       <right style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </right>
       <top style="thin">
-        <color indexed="22"/>
+        <color indexed="23"/>
       </top>
       <bottom style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </left>
       <right style="thin">
-        <color indexed="21"/>
+        <color indexed="23"/>
       </right>
       <top style="thin">
-        <color indexed="22"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="21"/>
+        <color indexed="23"/>
       </left>
       <right style="thin">
         <color indexed="22"/>
@@ -575,7 +629,7 @@
         <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </bottom>
       <diagonal/>
     </border>
@@ -584,43 +638,13 @@
         <color indexed="22"/>
       </left>
       <right style="thin">
-        <color indexed="21"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="21"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="21"/>
-      </left>
-      <right style="thin">
-        <color indexed="21"/>
-      </right>
-      <top style="thin">
-        <color indexed="21"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="21"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="21"/>
-      </left>
-      <right style="thin">
         <color indexed="22"/>
       </right>
       <top style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </top>
       <bottom style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </bottom>
       <diagonal/>
     </border>
@@ -629,13 +653,28 @@
         <color indexed="22"/>
       </left>
       <right style="thin">
-        <color indexed="21"/>
+        <color indexed="23"/>
       </right>
       <top style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
       </top>
       <bottom style="thin">
-        <color indexed="21"/>
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="23"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
       </bottom>
       <diagonal/>
     </border>
@@ -697,8 +736,8 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -733,7 +772,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -786,6 +825,7 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ff0000ee"/>
       <rgbColor rgb="ffcacaca"/>
       <rgbColor rgb="ffe6e6e6"/>
       <rgbColor rgb="ffbdc0bf"/>
@@ -1898,7 +1938,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s" s="3">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1909,12 +1949,12 @@
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s" s="3">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1925,7 +1965,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1945,7 +1985,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1980,20 +2020,30 @@
       <c r="E2" s="15"/>
     </row>
     <row r="3" ht="16.55" customHeight="1">
-      <c r="A3" t="s" s="16">
+      <c r="A3" t="s" s="11">
         <v>9</v>
       </c>
-      <c r="B3" t="s" s="17">
+      <c r="B3" t="s" s="12">
         <v>10</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" ht="16.55" customHeight="1">
+      <c r="A4" t="s" s="16">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s" s="17">
+        <v>12</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" location="" tooltip="" display="http://www.tanklib.franklidev.com/"/>
-    <hyperlink ref="B3" r:id="rId2" location="" tooltip="" display="http://www.tanklib.franklidev.com/"/>
+    <hyperlink ref="B4" r:id="rId1" location="" tooltip="" display="http://www.tanklib.franklidev.com/Page"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -2005,7 +2055,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2020,13 +2070,13 @@
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
       <c r="A1" t="s" s="22">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s" s="22">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s" s="22">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
@@ -2035,13 +2085,13 @@
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" t="s" s="24">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s" s="24">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s" s="24">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="25"/>
       <c r="E2" s="25"/>
@@ -2050,13 +2100,13 @@
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" t="s" s="22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s" s="22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s" s="22">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="23"/>
@@ -2065,13 +2115,13 @@
     </row>
     <row r="4" ht="20.25" customHeight="1">
       <c r="A4" t="s" s="24">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s" s="24">
         <v>21</v>
       </c>
-      <c r="B4" t="s" s="24">
-        <v>19</v>
-      </c>
       <c r="C4" t="s" s="24">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
@@ -2080,13 +2130,13 @@
     </row>
     <row r="5" ht="20.25" customHeight="1">
       <c r="A5" t="s" s="22">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s" s="22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s" s="22">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
@@ -2095,13 +2145,13 @@
     </row>
     <row r="6" ht="20.25" customHeight="1">
       <c r="A6" t="s" s="24">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s" s="24">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s" s="24">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
@@ -2110,13 +2160,13 @@
     </row>
     <row r="7" ht="20.25" customHeight="1">
       <c r="A7" t="s" s="22">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s" s="22">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s" s="22">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
@@ -2125,13 +2175,13 @@
     </row>
     <row r="8" ht="20.25" customHeight="1">
       <c r="A8" t="s" s="24">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s" s="24">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s" s="24">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D8" s="25"/>
       <c r="E8" s="25"/>
@@ -2140,13 +2190,13 @@
     </row>
     <row r="9" ht="20.25" customHeight="1">
       <c r="A9" t="s" s="22">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s" s="22">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
@@ -2155,13 +2205,13 @@
     </row>
     <row r="10" ht="20.25" customHeight="1">
       <c r="A10" t="s" s="24">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s" s="24">
         <v>34</v>
       </c>
-      <c r="B10" t="s" s="24">
-        <v>32</v>
-      </c>
       <c r="C10" t="s" s="24">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -2170,13 +2220,13 @@
     </row>
     <row r="11" ht="20.25" customHeight="1">
       <c r="A11" t="s" s="22">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s" s="22">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -2185,13 +2235,13 @@
     </row>
     <row r="12" ht="20.25" customHeight="1">
       <c r="A12" t="s" s="24">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s" s="24">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s" s="24">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -2200,13 +2250,13 @@
     </row>
     <row r="13" ht="20.25" customHeight="1">
       <c r="A13" t="s" s="22">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s" s="22">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
@@ -2215,13 +2265,13 @@
     </row>
     <row r="14" ht="20.25" customHeight="1">
       <c r="A14" t="s" s="24">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s" s="24">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s" s="24">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="25"/>
@@ -2230,13 +2280,13 @@
     </row>
     <row r="15" ht="20.25" customHeight="1">
       <c r="A15" t="s" s="22">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s" s="22">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -2245,13 +2295,13 @@
     </row>
     <row r="16" ht="20.25" customHeight="1">
       <c r="A16" t="s" s="24">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s" s="24">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s" s="24">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
@@ -2260,18 +2310,63 @@
     </row>
     <row r="17" ht="20.25" customHeight="1">
       <c r="A17" t="s" s="22">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s" s="22">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s" s="22">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
       <c r="F17" s="23"/>
       <c r="G17" s="23"/>
+    </row>
+    <row r="18" ht="20.25" customHeight="1">
+      <c r="A18" t="s" s="24">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s" s="24">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s" s="24">
+        <v>54</v>
+      </c>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+    </row>
+    <row r="19" ht="20.25" customHeight="1">
+      <c r="A19" t="s" s="22">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s" s="22">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s" s="22">
+        <v>56</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+    </row>
+    <row r="20" ht="20.25" customHeight="1">
+      <c r="A20" t="s" s="24">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s" s="24">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s" s="24">
+        <v>58</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -2303,10 +2398,10 @@
   <sheetData>
     <row r="1" ht="14.35" customHeight="1">
       <c r="A1" t="s" s="27">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s" s="27">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -2314,10 +2409,10 @@
     </row>
     <row r="2" ht="14.7" customHeight="1">
       <c r="A2" t="s" s="29">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s" s="30">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="32"/>

</xml_diff>

<commit_message>
Adjust AddTank test to support ResetData
Support testing on MaxRecordCountReached case which displays a modal view to urge the user to reset data instead of displaying the edit page
</commit_message>
<xml_diff>
--- a/TestOnTankLibrary/Data/Location.xlsx
+++ b/TestOnTankLibrary/Data/Location.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -100,7 +100,7 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Home.AddTank</t>
+    <t>Home.AddTank.Add</t>
   </si>
   <si>
     <t>CssSelector</t>
@@ -224,6 +224,24 @@
   </si>
   <si>
     <t>//a[text()='Back to List']</t>
+  </si>
+  <si>
+    <t>Home.AddTank.ResetData</t>
+  </si>
+  <si>
+    <t>//div[@id='ResetData']//a[text()='Reset Data']</t>
+  </si>
+  <si>
+    <t>Home.AddTank.ResetModal</t>
+  </si>
+  <si>
+    <t>//div[@id='ResetData']</t>
+  </si>
+  <si>
+    <t>Home.AddTank.CloseModal</t>
+  </si>
+  <si>
+    <t>//div[@id='ResetData']//a[text()='Close']</t>
   </si>
   <si>
     <t>Expected</t>
@@ -1954,7 +1972,7 @@
     </row>
     <row r="13">
       <c r="B13" t="s" s="3">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -1965,7 +1983,7 @@
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2055,7 +2073,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2367,6 +2385,51 @@
       <c r="E20" s="25"/>
       <c r="F20" s="25"/>
       <c r="G20" s="25"/>
+    </row>
+    <row r="21" ht="20.25" customHeight="1">
+      <c r="A21" t="s" s="22">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s" s="22">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s" s="22">
+        <v>60</v>
+      </c>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+    </row>
+    <row r="22" ht="20.25" customHeight="1">
+      <c r="A22" t="s" s="24">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s" s="24">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s" s="24">
+        <v>62</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+    </row>
+    <row r="23" ht="20.25" customHeight="1">
+      <c r="A23" t="s" s="22">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s" s="22">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s" s="22">
+        <v>64</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
@@ -2401,7 +2464,7 @@
         <v>14</v>
       </c>
       <c r="B1" t="s" s="27">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -2409,10 +2472,10 @@
     </row>
     <row r="2" ht="14.7" customHeight="1">
       <c r="A2" t="s" s="29">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s" s="30">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="32"/>

</xml_diff>